<commit_message>
add 유저 기능, add Jwt config 파일, add 기타 config 파일, add swagger config파일
</commit_message>
<xml_diff>
--- a/BackEnd/src/main/resources/res/api_specification.xlsx
+++ b/BackEnd/src/main/resources/res/api_specification.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="129">
   <si>
     <t xml:space="preserve">서비스</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">/user/login</t>
   </si>
   <si>
-    <t xml:space="preserve">{"user_id": "", "user_pwd": ""}</t>
+    <t xml:space="preserve">{“user_id”: “”, “user_pwd”: “”}</t>
   </si>
   <si>
     <t xml:space="preserve">로그아웃</t>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">/user/logout</t>
   </si>
   <si>
+    <t xml:space="preserve">{“user_id”: “”}</t>
+  </si>
+  <si>
     <t xml:space="preserve">회원 가입</t>
   </si>
   <si>
@@ -82,9 +85,6 @@
     <t xml:space="preserve">{“user_name”: “”, "user_email": ""}</t>
   </si>
   <si>
-    <t xml:space="preserve">{“user_id”: “”}</t>
-  </si>
-  <si>
     <t xml:space="preserve">?</t>
   </si>
   <si>
@@ -100,13 +100,16 @@
     <t xml:space="preserve">{“user_pwd”: “”}</t>
   </si>
   <si>
+    <t xml:space="preserve">미구현</t>
+  </si>
+  <si>
     <t xml:space="preserve">계정 중복 확인</t>
   </si>
   <si>
     <t xml:space="preserve">GET</t>
   </si>
   <si>
-    <t xml:space="preserve">/user/check/${id}</t>
+    <t xml:space="preserve">/user/check/${user_id}</t>
   </si>
   <si>
     <t xml:space="preserve">{"user_id": ""}</t>
@@ -118,7 +121,7 @@
     <t xml:space="preserve">/user/check/password</t>
   </si>
   <si>
-    <t xml:space="preserve">{"user_pwd": ""}</t>
+    <t xml:space="preserve">{“user_id”: “”, "user_pwd": ""}</t>
   </si>
   <si>
     <t xml:space="preserve">회원 정보 수정</t>
@@ -130,7 +133,7 @@
     <t xml:space="preserve">/user/change</t>
   </si>
   <si>
-    <t xml:space="preserve">{user_name": "", "user_address": "", "user_email": ""}</t>
+    <t xml:space="preserve">{“user_id”: “”, user_name": "", "user_address": "", "user_email": ""}</t>
   </si>
   <si>
     <t xml:space="preserve">비밀번호 수정</t>
@@ -139,6 +142,9 @@
     <t xml:space="preserve">/user/change/password</t>
   </si>
   <si>
+    <t xml:space="preserve">{“user_id”: “”, “user_pwd”: “”, “new_user_pwd”: “”}</t>
+  </si>
+  <si>
     <t xml:space="preserve">회원 정보 조회</t>
   </si>
   <si>
@@ -157,6 +163,18 @@
     <t xml:space="preserve">/user/delete</t>
   </si>
   <si>
+    <t xml:space="preserve">인증</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/user/authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access Token 재발급</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/user/reissue</t>
+  </si>
+  <si>
     <t xml:space="preserve">회원 목록 조회</t>
   </si>
   <si>
@@ -166,40 +184,13 @@
     <t xml:space="preserve">[{"user_id": "", "user_name": "", "user_address": "", "user_email": ""}]</t>
   </si>
   <si>
-    <t xml:space="preserve">회원 조회(by 사용자 계정)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/admin/user/{user_id}</t>
+    <t xml:space="preserve">회원 목록 조회(조건)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/admin/user/{attribute}</t>
   </si>
   <si>
     <t xml:space="preserve">{"user_id": "", "user_name": "", "user_address": "", "user_email": ""}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">회원 조회(by 사용자 이름)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/admin/user/{user_name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{“user_name”: “”}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">회원 조회(by 사용자 거주지)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/admin/user/{user_address}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{“user_address”: “”}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">회원 조회(by 사용자 이메일)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/admin/user/{user_email}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{“user_email”: “”}</t>
   </si>
   <si>
     <t xml:space="preserve">house</t>
@@ -489,7 +480,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,6 +503,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEBCD"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -610,7 +607,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -639,10 +636,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -671,15 +664,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -769,10 +770,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:H46"/>
+  <dimension ref="A2:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,7 +843,9 @@
       <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
@@ -850,16 +853,16 @@
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -868,19 +871,19 @@
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>21</v>
@@ -904,24 +907,24 @@
       <c r="G7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>21</v>
+      <c r="H7" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -930,16 +933,16 @@
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5" t="s">
@@ -950,16 +953,16 @@
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -968,16 +971,16 @@
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -986,19 +989,19 @@
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>21</v>
@@ -1008,639 +1011,624 @@
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6" t="s">
+      <c r="G17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="C18" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="D18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7" t="s">
+      <c r="F18" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="G18" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="H18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="8" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="D19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>65</v>
       </c>
+      <c r="G19" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="8"/>
+      <c r="G20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8" t="s">
+      <c r="H21" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="8" t="s">
+      <c r="C22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="D22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="8" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
+      <c r="D24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10" t="s">
+      <c r="F24" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="C25" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="10" t="s">
+      <c r="E26" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="F26" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="12" t="s">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="12"/>
+      <c r="C27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12" t="s">
+      <c r="D27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="F27" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="14"/>
+      <c r="C29" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="12" t="s">
+      <c r="E29" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="14" t="s">
+      <c r="F29" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="14"/>
+      <c r="C30" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13"/>
-      <c r="C30" s="14" t="s">
+      <c r="D30" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="13"/>
-      <c r="C31" s="14" t="s">
+      <c r="D31" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>96</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>92</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="G31" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13"/>
-      <c r="C32" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="14" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="D32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="14"/>
+      <c r="C33" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="D33" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13"/>
-      <c r="C33" s="14" t="s">
+      <c r="F33" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="13"/>
-      <c r="C34" s="14" t="s">
+      <c r="D34" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="14" t="s">
+      <c r="F34" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="13"/>
-      <c r="C35" s="14" t="s">
+      <c r="G34" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="C35" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="D35" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="G35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="15"/>
+      <c r="F35" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="17" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="17" t="s">
+      <c r="D36" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G36" s="17" t="s">
+      <c r="F36" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="H36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17" t="s">
+      <c r="B37" s="17"/>
+      <c r="C37" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4"/>
+      <c r="C40" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="16"/>
-      <c r="C38" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="16"/>
-      <c r="C39" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="F39" s="17" t="s">
+      <c r="E40" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19" t="s">
-        <v>93</v>
-      </c>
+      <c r="F40" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="19"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="4"/>
-      <c r="C41" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
+      <c r="C41" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="4"/>
-      <c r="C42" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="18" t="s">
+      <c r="C42" s="19" t="s">
         <v>122</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
+      <c r="G42" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H42" s="19"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="4"/>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="19"/>
+      <c r="H43" s="20"/>
+    </row>
+    <row r="44" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4"/>
+      <c r="C44" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="18" t="s">
+      <c r="D44" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H43" s="18"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="4"/>
-      <c r="C44" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G44" s="18"/>
-      <c r="H44" s="19"/>
+      <c r="F44" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="4"/>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="H45" s="19"/>
-    </row>
-    <row r="46" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="4"/>
-      <c r="C46" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="H46" s="19"/>
-    </row>
+      <c r="F45" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H45" s="20"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B3:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="B3:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B45"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fix controller mapping path
</commit_message>
<xml_diff>
--- a/BackEnd/src/main/resources/res/api_specification.xlsx
+++ b/BackEnd/src/main/resources/res/api_specification.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="140">
   <si>
     <t>서비스</t>
   </si>
@@ -377,9 +377,6 @@
     <t>댓글 작성</t>
   </si>
   <si>
-    <t>/comment</t>
-  </si>
-  <si>
     <t>{“user_id”: “”, “article_no”: , “content”: “”}</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t>댓글 삭제</t>
   </si>
   <si>
-    <t>/comment/{comment_id}</t>
-  </si>
-  <si>
     <t>{“comment_id”: }</t>
   </si>
   <si>
@@ -435,6 +429,26 @@
   </si>
   <si>
     <t>POST</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/delete/{article_no}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/notice/delete/{article_no}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comment/write</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comment/modify</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comment/delete/{comment_id}</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -613,65 +627,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1024,818 +1038,818 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="46.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="17.875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="75" style="7" customWidth="1"/>
-    <col min="7" max="7" width="171.625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="52.625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="171.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="10" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="10" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="10" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="10" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="10" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="10" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="10" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="10" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="10" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="12" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12" t="s">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="12" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B18" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+      <c r="C20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="C21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B22" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
+      <c r="C23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B24" s="18"/>
+      <c r="C24" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B25" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B26" s="19"/>
+      <c r="C26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B27" s="19"/>
+      <c r="C27" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B28" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B29" s="20"/>
+      <c r="C29" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B30" s="20"/>
+      <c r="C30" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B31" s="20"/>
+      <c r="C31" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B32" s="20"/>
+      <c r="C32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B33" s="20"/>
+      <c r="C33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B34" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B35" s="15"/>
+      <c r="C35" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B36" s="15"/>
+      <c r="C36" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+    </row>
+    <row r="37" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B37" s="15"/>
+      <c r="C37" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B38" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B39" s="16"/>
+      <c r="C39" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B40" s="16"/>
+      <c r="C40" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B41" s="16"/>
+      <c r="C41" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B42" s="16"/>
+      <c r="C42" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-      <c r="C19" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
-      <c r="C20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="14"/>
-    </row>
-    <row r="23" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
-      <c r="C24" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B27" s="3"/>
-      <c r="C27" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17" t="s">
+      <c r="F42" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B43" s="16"/>
+      <c r="C43" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G43" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="H28" s="17"/>
-    </row>
-    <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-      <c r="C29" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
-      <c r="C30" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
-      <c r="C31" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-      <c r="C32" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="17"/>
-    </row>
-    <row r="33" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="C33" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="H34" s="18"/>
-    </row>
-    <row r="35" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
-      <c r="C35" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
-      <c r="C36" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-    </row>
-    <row r="37" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B37" s="1"/>
-      <c r="C37" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-    </row>
-    <row r="38" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B38" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
-      <c r="C39" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-    </row>
-    <row r="40" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
-      <c r="C40" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-    </row>
-    <row r="41" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B41" s="6"/>
-      <c r="C41" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H41" s="19"/>
-    </row>
-    <row r="42" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B42" s="6"/>
-      <c r="C42" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="20"/>
-    </row>
-    <row r="43" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B43" s="6"/>
-      <c r="C43" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H43" s="20"/>
+      <c r="H43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
modify 공지사항 및 글 조회 Mapping path
</commit_message>
<xml_diff>
--- a/BackEnd/src/main/resources/res/api_specification.xlsx
+++ b/BackEnd/src/main/resources/res/api_specification.xlsx
@@ -338,9 +338,6 @@
     <t>게시판 글 조회</t>
   </si>
   <si>
-    <t>/board/search/{article_no}</t>
-  </si>
-  <si>
     <t>{“article_no”: ""}</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
   </si>
   <si>
     <t>공지사항 조회</t>
-  </si>
-  <si>
-    <t>/notice/search/{article_no}</t>
   </si>
   <si>
     <t>공지사항 삭제</t>
@@ -449,6 +443,14 @@
   </si>
   <si>
     <t>/comment/delete/{comment_id}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/view/{article_no}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>/notice/view/{article_no}</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1038,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1360,7 @@
         <v>56</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>57</v>
@@ -1379,7 +1381,7 @@
         <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>61</v>
@@ -1625,29 +1627,29 @@
         <v>28</v>
       </c>
       <c r="E31" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="G31" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B32" s="20"/>
       <c r="C32" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="11"/>
@@ -1655,16 +1657,16 @@
     <row r="33" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B33" s="20"/>
       <c r="C33" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E33" s="10" t="s">
+      <c r="F33" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>96</v>
@@ -1673,38 +1675,38 @@
     </row>
     <row r="34" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="G34" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>115</v>
       </c>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B35" s="15"/>
       <c r="C35" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -1712,16 +1714,16 @@
     <row r="36" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B36" s="15"/>
       <c r="C36" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
@@ -1729,32 +1731,32 @@
     <row r="37" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B37" s="15"/>
       <c r="C37" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B38" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="14" t="s">
@@ -1765,13 +1767,13 @@
     <row r="39" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B39" s="16"/>
       <c r="C39" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F39" s="14" t="s">
         <v>99</v>
@@ -1782,13 +1784,13 @@
     <row r="40" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B40" s="16"/>
       <c r="C40" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>35</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>102</v>
@@ -1799,35 +1801,35 @@
     <row r="41" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B41" s="16"/>
       <c r="C41" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B42" s="16"/>
       <c r="C42" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>45</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G42" s="13"/>
       <c r="H42" s="14"/>
@@ -1835,16 +1837,16 @@
     <row r="43" spans="2:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B43" s="16"/>
       <c r="C43" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>134</v>
-      </c>
       <c r="E43" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G43" s="14" t="s">
         <v>96</v>

</xml_diff>